<commit_message>
Incremental Global Exception Handling
</commit_message>
<xml_diff>
--- a/docs/Phase1_UseCases.xlsx
+++ b/docs/Phase1_UseCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="14685"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="14690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Role</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Get a Task History Report</t>
+  </si>
+  <si>
+    <t>See a List of Tasks By Status</t>
   </si>
 </sst>
 </file>
@@ -442,25 +445,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,7 +477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -488,40 +491,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -529,16 +517,22 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
       <c r="I5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -547,18 +541,15 @@
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -567,13 +558,18 @@
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -581,13 +577,14 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -595,10 +592,13 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -607,27 +607,38 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented PUT with status transitions. Also CORs for the Web API.
</commit_message>
<xml_diff>
--- a/docs/Phase1_UseCases.xlsx
+++ b/docs/Phase1_UseCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Role</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Archive</t>
-  </si>
-  <si>
-    <t>InProgress</t>
   </si>
   <si>
     <t>Creates a New Backlog Task</t>
@@ -447,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,23 +485,23 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -515,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -524,58 +521,58 @@
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -584,62 +581,59 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>